<commit_message>
EPS (and now also SVG) export changed to Batik (from epsgraphics), removing questionable dependency on GPL-licenced software
</commit_message>
<xml_diff>
--- a/groove/trunk/src/meta/libraries.xlsx
+++ b/groove/trunk/src/meta/libraries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2023-03\groove\src\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B5DDFF-A15B-4617-AD62-A973E0270864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EAFD4-6ECE-4662-A060-B9CAFF36454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21855" yWindow="2295" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="3150" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="libraries" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>Antlr</t>
   </si>
@@ -151,15 +151,6 @@
     <t>2.7.0</t>
   </si>
   <si>
-    <t>EPSGraphics</t>
-  </si>
-  <si>
-    <t>exporting displayed graphs to EPS format</t>
-  </si>
-  <si>
-    <t>http://www.abeel.be/epsgraphics/</t>
-  </si>
-  <si>
     <t>1.2</t>
   </si>
   <si>
@@ -343,9 +334,6 @@
     <t>https://javaee.github.io/jaxb-v2/</t>
   </si>
   <si>
-    <t>GPL 2.0</t>
-  </si>
-  <si>
     <t>MIT</t>
   </si>
   <si>
@@ -370,9 +358,6 @@
     <t>NOSA 1.3</t>
   </si>
   <si>
-    <t>https://wiki.eclipse.org/JDT_Core/Null_Analysis/External_Annotations</t>
-  </si>
-  <si>
     <t>access to an XML document from a Java program</t>
   </si>
   <si>
@@ -389,6 +374,24 @@
   </si>
   <si>
     <t>https://github.com/esb-lwb/lwb</t>
+  </si>
+  <si>
+    <t>https://wiki.eclipse.org/JDT_Core/Null_Analysis</t>
+  </si>
+  <si>
+    <t>Batik</t>
+  </si>
+  <si>
+    <t>exporting images to SVG, EPS, …</t>
+  </si>
+  <si>
+    <t>https://xmlgraphics.apache.org/batik/</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>CDDL 1.1 or GPL 2.0 with classpath exception</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,19 +1269,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1292,10 +1295,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,41 +1315,41 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
         <v>81</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,245 +1366,245 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>45</v>
-      </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -1685,7 +1688,7 @@
       </c>
       <c r="C4" t="str">
         <f>libraries!C5</f>
-        <v>https://wiki.eclipse.org/JDT_Core/Null_Analysis/External_Annotations</v>
+        <v>https://wiki.eclipse.org/JDT_Core/Null_Analysis</v>
       </c>
       <c r="D4" t="str">
         <f>libraries!D5</f>
@@ -1711,21 +1714,21 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>libraries!A7</f>
-        <v>EPSGraphics</v>
-      </c>
-      <c r="B6" t="str">
-        <f>libraries!B7</f>
-        <v>exporting displayed graphs to EPS format</v>
-      </c>
-      <c r="C6" t="str">
-        <f>libraries!C7</f>
-        <v>http://www.abeel.be/epsgraphics/</v>
-      </c>
-      <c r="D6" t="str">
-        <f>libraries!D7</f>
-        <v>1.2</v>
+      <c r="A6" t="e">
+        <f>libraries!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B6" t="e">
+        <f>libraries!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C6" t="e">
+        <f>libraries!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D6" t="e">
+        <f>libraries!#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved type derivation for fields in expressions and assignments (for typed rule systems)
</commit_message>
<xml_diff>
--- a/groove/trunk/src/meta/libraries.xlsx
+++ b/groove/trunk/src/meta/libraries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2023-03\groove\src\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2022-09\groove\src\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EAFD4-6ECE-4662-A060-B9CAFF36454C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A461728A-BDAB-4F68-9135-23CA3E352898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="3150" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="libraries" sheetId="1" r:id="rId1"/>
@@ -1255,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,21 +1714,21 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="e">
-        <f>libraries!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B6" t="e">
-        <f>libraries!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C6" t="e">
-        <f>libraries!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" t="e">
-        <f>libraries!#REF!</f>
-        <v>#REF!</v>
+      <c r="A6" t="str">
+        <f>libraries!A7</f>
+        <v>Batik</v>
+      </c>
+      <c r="B6" t="str">
+        <f>libraries!B7</f>
+        <v>exporting images to SVG, EPS, …</v>
+      </c>
+      <c r="C6" t="str">
+        <f>libraries!C7</f>
+        <v>https://xmlgraphics.apache.org/batik/</v>
+      </c>
+      <c r="D6" t="str">
+        <f>libraries!D7</f>
+        <v>1.17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced iTextPdf library by Apache FOP (to escape AGPL license)
</commit_message>
<xml_diff>
--- a/groove/trunk/src/meta/libraries.xlsx
+++ b/groove/trunk/src/meta/libraries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2022-09\groove\src\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2023-03\groove\src\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A461728A-BDAB-4F68-9135-23CA3E352898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9A171-6838-48C7-8722-3FFE509D4770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="3150" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="libraries" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>Antlr</t>
   </si>
@@ -178,18 +178,9 @@
     <t>2.0.5</t>
   </si>
   <si>
-    <t>iText</t>
-  </si>
-  <si>
     <t>exporting displayed graphs to PDF format</t>
   </si>
   <si>
-    <t>http://itextpdf.com/</t>
-  </si>
-  <si>
-    <t>5.3.2</t>
-  </si>
-  <si>
     <t>JGoodies Looks</t>
   </si>
   <si>
@@ -340,9 +331,6 @@
     <t>BSD</t>
   </si>
   <si>
-    <t>AGPL 3.0</t>
-  </si>
-  <si>
     <t>BSD 3-clause</t>
   </si>
   <si>
@@ -379,9 +367,6 @@
     <t>https://wiki.eclipse.org/JDT_Core/Null_Analysis</t>
   </si>
   <si>
-    <t>Batik</t>
-  </si>
-  <si>
     <t>exporting images to SVG, EPS, …</t>
   </si>
   <si>
@@ -392,6 +377,18 @@
   </si>
   <si>
     <t>CDDL 1.1 or GPL 2.0 with classpath exception</t>
+  </si>
+  <si>
+    <t>Apache Batik</t>
+  </si>
+  <si>
+    <t>Apache FOP</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>https://xmlgraphics.apache.org/fop/</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1253,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,19 +1266,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1295,95 +1292,95 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,7 +1397,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,194 +1414,194 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1618,7 +1615,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,91 +1641,91 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>libraries!A3</f>
-        <v>Args4J</v>
+        <v>Apache Batik</v>
       </c>
       <c r="B2" t="str">
         <f>libraries!B3</f>
-        <v>command-line option parsing</v>
+        <v>exporting images to SVG, EPS, …</v>
       </c>
       <c r="C2" t="str">
         <f>libraries!C3</f>
-        <v>http://args4j.kohsuke.org/</v>
+        <v>https://xmlgraphics.apache.org/batik/</v>
       </c>
       <c r="D2" t="str">
         <f>libraries!D3</f>
-        <v>2.0.26</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>libraries!A4</f>
-        <v>JAXB</v>
+        <v>Apache FOP</v>
       </c>
       <c r="B3" t="str">
         <f>libraries!B4</f>
-        <v>access to an XML document from a Java program</v>
+        <v>exporting displayed graphs to PDF format</v>
       </c>
       <c r="C3" t="str">
         <f>libraries!C4</f>
-        <v>https://javaee.github.io/jaxb-v2/</v>
+        <v>https://xmlgraphics.apache.org/fop/</v>
       </c>
       <c r="D3" t="str">
         <f>libraries!D4</f>
-        <v>3.0.2</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>libraries!A5</f>
-        <v>Java Annotations</v>
+        <v>Args4J</v>
       </c>
       <c r="B4" t="str">
         <f>libraries!B5</f>
-        <v>runtime analysis of Java annotations</v>
+        <v>command-line option parsing</v>
       </c>
       <c r="C4" t="str">
         <f>libraries!C5</f>
-        <v>https://wiki.eclipse.org/JDT_Core/Null_Analysis</v>
+        <v>http://args4j.kohsuke.org/</v>
       </c>
       <c r="D4" t="str">
         <f>libraries!D5</f>
-        <v>2.2.700</v>
+        <v>2.0.26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>libraries!A6</f>
-        <v>EMF</v>
+        <v>JAXB</v>
       </c>
       <c r="B5" t="str">
         <f>libraries!B6</f>
-        <v>converting to and from Eclipse ecore format</v>
+        <v>access to an XML document from a Java program</v>
       </c>
       <c r="C5" t="str">
         <f>libraries!C6</f>
-        <v>http://eclipse.org</v>
+        <v>https://javaee.github.io/jaxb-v2/</v>
       </c>
       <c r="D5" t="str">
         <f>libraries!D6</f>
-        <v>2.7.0</v>
+        <v>3.0.2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>libraries!A7</f>
-        <v>Batik</v>
+        <v>EMF</v>
       </c>
       <c r="B6" t="str">
         <f>libraries!B7</f>
-        <v>exporting images to SVG, EPS, …</v>
+        <v>converting to and from Eclipse ecore format</v>
       </c>
       <c r="C6" t="str">
         <f>libraries!C7</f>
-        <v>https://xmlgraphics.apache.org/batik/</v>
+        <v>http://eclipse.org</v>
       </c>
       <c r="D6" t="str">
         <f>libraries!D7</f>
-        <v>1.17</v>
+        <v>2.7.0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1770,55 +1767,55 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>libraries!A10</f>
-        <v>iText</v>
+        <v>Jakarta activation</v>
       </c>
       <c r="B9" t="str">
         <f>libraries!B10</f>
-        <v>exporting displayed graphs to PDF format</v>
+        <v>dynamic data manipulation</v>
       </c>
       <c r="C9" t="str">
         <f>libraries!C10</f>
-        <v>http://itextpdf.com/</v>
+        <v>https://projects.eclipse.org/projects/ee4j.jaf</v>
       </c>
       <c r="D9" t="str">
         <f>libraries!D10</f>
-        <v>5.3.2</v>
+        <v>3.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>libraries!A11</f>
-        <v>Jakarta activation</v>
+        <v>Jakarta bind</v>
       </c>
       <c r="B10" t="str">
         <f>libraries!B11</f>
-        <v>dynamic data manipulation</v>
+        <v>mapping between XML documents and Java objects</v>
       </c>
       <c r="C10" t="str">
         <f>libraries!C11</f>
-        <v>https://projects.eclipse.org/projects/ee4j.jaf</v>
+        <v>https://jakarta.ee/specifications/xml-binding/</v>
       </c>
       <c r="D10" t="str">
         <f>libraries!D11</f>
-        <v>3.0.1</v>
+        <v>1.2.2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>libraries!A12</f>
-        <v>Jakarta bind</v>
+        <v>Java Annotations</v>
       </c>
       <c r="B11" t="str">
         <f>libraries!B12</f>
-        <v>mapping between XML documents and Java objects</v>
+        <v>runtime analysis of Java annotations</v>
       </c>
       <c r="C11" t="str">
         <f>libraries!C12</f>
-        <v>https://jakarta.ee/specifications/xml-binding/</v>
+        <v>https://wiki.eclipse.org/JDT_Core/Null_Analysis</v>
       </c>
       <c r="D11" t="str">
         <f>libraries!D12</f>
-        <v>1.2.2</v>
+        <v>2.2.700</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Version files in the resource directory rather than hardcoded in the Version class
</commit_message>
<xml_diff>
--- a/groove/trunk/src/meta/libraries.xlsx
+++ b/groove/trunk/src/meta/libraries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2023-03\groove\src\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9A171-6838-48C7-8722-3FFE509D4770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FE6D70-E0F6-47CA-9CBE-24CEFAB3B140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="3150" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="libraries" sheetId="1" r:id="rId1"/>
@@ -367,9 +367,6 @@
     <t>https://wiki.eclipse.org/JDT_Core/Null_Analysis</t>
   </si>
   <si>
-    <t>exporting images to SVG, EPS, …</t>
-  </si>
-  <si>
     <t>https://xmlgraphics.apache.org/batik/</t>
   </si>
   <si>
@@ -389,6 +386,9 @@
   </si>
   <si>
     <t>https://xmlgraphics.apache.org/fop/</t>
+  </si>
+  <si>
+    <t>exporting images to SVG, EPS, ...</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,16 +1300,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -1317,16 +1317,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" t="s">
         <v>55</v>
@@ -1363,7 +1363,7 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,11 +1614,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -1645,7 +1649,7 @@
       </c>
       <c r="B2" t="str">
         <f>libraries!B3</f>
-        <v>exporting images to SVG, EPS, …</v>
+        <v>exporting images to SVG, EPS, ...</v>
       </c>
       <c r="C2" t="str">
         <f>libraries!C3</f>

</xml_diff>